<commit_message>
helpful print statements for run_mislabel_sim
</commit_message>
<xml_diff>
--- a/simulations/tests/sample_genotype_data_tests.xlsx
+++ b/simulations/tests/sample_genotype_data_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlesdeng/Workspace/mislabeling/simulations/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121833B6-CA82-CE44-B5C1-AFAB2A952BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80642E9-D2C1-BD46-864D-8454D523829E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="740" windowWidth="12780" windowHeight="17140" firstSheet="3" activeTab="9" xr2:uid="{24718B40-BA6E-C848-85FD-DBE914F41A4D}"/>
+    <workbookView xWindow="2280" yWindow="740" windowWidth="12780" windowHeight="17000" firstSheet="6" activeTab="9" xr2:uid="{24718B40-BA6E-C848-85FD-DBE914F41A4D}"/>
   </bookViews>
   <sheets>
     <sheet name="1-4C-1-3C-1-2C-2G" sheetId="16" r:id="rId1"/>
@@ -966,7 +966,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
make more memory efficient
</commit_message>
<xml_diff>
--- a/simulations/tests/sample_genotype_data_tests.xlsx
+++ b/simulations/tests/sample_genotype_data_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlesdeng/Workspace/mislabeling/simulations/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8444A99-5134-3941-BDCE-D201FFB86CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DF4F74-E624-0942-8744-138274533902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" firstSheet="6" activeTab="7" xr2:uid="{24718B40-BA6E-C848-85FD-DBE914F41A4D}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17000" firstSheet="8" activeTab="19" xr2:uid="{24718B40-BA6E-C848-85FD-DBE914F41A4D}"/>
   </bookViews>
   <sheets>
     <sheet name="1-4C-1-3C-1-2C-2G" sheetId="16" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <sheet name="1-2C-D" sheetId="3" r:id="rId17"/>
     <sheet name="Maj_Edge_Case" sheetId="4" r:id="rId18"/>
     <sheet name="2-2C_Edge_Case" sheetId="5" r:id="rId19"/>
+    <sheet name="3C-D" sheetId="22" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="108">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -341,6 +342,42 @@
   </si>
   <si>
     <t>Bill_1 - Andy_3 - Chris_2</t>
+  </si>
+  <si>
+    <t>Case0127_Sample1</t>
+  </si>
+  <si>
+    <t>Case0127_Sample2</t>
+  </si>
+  <si>
+    <t>Case0127_Sample3</t>
+  </si>
+  <si>
+    <t>Ctrl1270_Sample1</t>
+  </si>
+  <si>
+    <t>Ctrl1270_Sample2</t>
+  </si>
+  <si>
+    <t>Ctrl0305_Sample1</t>
+  </si>
+  <si>
+    <t>Ctrl0305_Sample3</t>
+  </si>
+  <si>
+    <t>Ctrl0305_Sample4</t>
+  </si>
+  <si>
+    <t>Ctrl0305_Sample5</t>
+  </si>
+  <si>
+    <t>Case0127</t>
+  </si>
+  <si>
+    <t>Ctrl1270</t>
+  </si>
+  <si>
+    <t>Ctrl0305</t>
   </si>
 </sst>
 </file>
@@ -401,6 +438,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>165099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>125522</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10A8850E-A88D-691F-068B-D224B849424E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="571499"/>
+          <a:ext cx="4711700" cy="5040423"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2671,7 +2757,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3021,6 +3107,135 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0BD89D7-EDF2-5743-935F-C268F844D4B9}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4050,7 +4265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{128533F5-440D-B34A-BAB9-65AE66BE3984}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>

</xml_diff>